<commit_message>
Refactor indicator logic and UI, add new indicators
Refactored indicator calculation and filtering logic for improved flexibility and accuracy. Added new indicators and adjusted existing ones in data processing and UI modules. Replaced cached data accessors with direct list-based retrieval. Updated sidebar and indicator modules to support new aggregation and filtering logic. Improved map and plot titles, and added spinner loading to charts. Updated dependencies and internal data structures to support these changes.
</commit_message>
<xml_diff>
--- a/inst/indicators.xlsx
+++ b/inst/indicators.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\moh.analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\moh.analytics\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D7397AF3-98D8-476B-987E-277DE23BA4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFDCC4A-9B28-4D36-B5CA-07A69AE89747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{6387D201-81FB-42D9-A202-087F66466527}"/>
+    <workbookView xWindow="1830" yWindow="1830" windowWidth="13116" windowHeight="8904" xr2:uid="{6387D201-81FB-42D9-A202-087F66466527}"/>
   </bookViews>
   <sheets>
     <sheet name="service" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="443">
   <si>
     <t>element_id</t>
   </si>
@@ -198,12 +198,6 @@
     <t>MOH 711 Normal Deliveries</t>
   </si>
   <si>
-    <t>Total Skilled Deliveries</t>
-  </si>
-  <si>
-    <t>sba</t>
-  </si>
-  <si>
     <t>rAZBTMa7Jy3</t>
   </si>
   <si>
@@ -291,9 +285,6 @@
     <t>MOH 706_Malaria BS (5 years and above) Number Positive</t>
   </si>
   <si>
-    <t>Confirmed malaria cases</t>
-  </si>
-  <si>
     <t>qi4TilPOx6o.nwpzSJ8o7hD</t>
   </si>
   <si>
@@ -396,9 +387,6 @@
     <t>Confirmed Malaria (only Positive cases)</t>
   </si>
   <si>
-    <t>Sum of Confirmed Malaria (only Positive cases) &lt;5 yrs and Confirmed Malaria (only Positive cases) &gt;5 yrs</t>
-  </si>
-  <si>
     <t>confirmed_malaria</t>
   </si>
   <si>
@@ -537,15 +525,6 @@
     <t>cbe</t>
   </si>
   <si>
-    <t>aq2ZahgvNWr</t>
-  </si>
-  <si>
-    <t>Outpatients with mental health conditions</t>
-  </si>
-  <si>
-    <t>Total Mental Disorders (&lt;&amp;&gt;5yrs)</t>
-  </si>
-  <si>
     <t>mental_disorder</t>
   </si>
   <si>
@@ -1240,6 +1219,138 @@
   </si>
   <si>
     <t>pop_15_24</t>
+  </si>
+  <si>
+    <t>csection</t>
+  </si>
+  <si>
+    <t>instdelivery</t>
+  </si>
+  <si>
+    <t>Institutional Delivery</t>
+  </si>
+  <si>
+    <t>Caeserean Section</t>
+  </si>
+  <si>
+    <t>IEfyuOqoU2d</t>
+  </si>
+  <si>
+    <t>MOH 717 Rev2020_No of Orthopeadic Cases assisted in theatre</t>
+  </si>
+  <si>
+    <t>Number of Orthopedic Cases assisted in theatre</t>
+  </si>
+  <si>
+    <t>ortho_assist</t>
+  </si>
+  <si>
+    <t>MqesiLWjOTS</t>
+  </si>
+  <si>
+    <t>Number of Emergency surgical cases operated on within one hour</t>
+  </si>
+  <si>
+    <t>Number of emergency surgical cases operated within 1 hour</t>
+  </si>
+  <si>
+    <t>surgial_emergency</t>
+  </si>
+  <si>
+    <t>MOH 731 Viral load &lt;1000_12mths HV03-042</t>
+  </si>
+  <si>
+    <t>RNfqUayuZP2</t>
+  </si>
+  <si>
+    <t>Number of patiently virally suppressed(&lt;1000 copies/ml) at 12 months</t>
+  </si>
+  <si>
+    <t>viral_suppressed</t>
+  </si>
+  <si>
+    <t>MOH 643C_VL Total Tests done</t>
+  </si>
+  <si>
+    <t>iiTUtZJWNT2</t>
+  </si>
+  <si>
+    <t>Number of patiently who had at least one VL test at 12 months</t>
+  </si>
+  <si>
+    <t>total_vl</t>
+  </si>
+  <si>
+    <t>Tf93vuu9qr5</t>
+  </si>
+  <si>
+    <t>MOH 643C F-CDRR for EID and Viral Load lab commodities</t>
+  </si>
+  <si>
+    <t>MOH 731-3 HIV and TB treatment Revision 2018</t>
+  </si>
+  <si>
+    <t>Vo4KDrUFwnA</t>
+  </si>
+  <si>
+    <t>hiv_treatment_rr</t>
+  </si>
+  <si>
+    <t>AWP Monthly Service Delivery</t>
+  </si>
+  <si>
+    <t>oVTOGGXwSVa</t>
+  </si>
+  <si>
+    <t>service_delivery_rr</t>
+  </si>
+  <si>
+    <t>Blood Slide Positive</t>
+  </si>
+  <si>
+    <t>Mental Disorders</t>
+  </si>
+  <si>
+    <t>HmgfJSVUOOr</t>
+  </si>
+  <si>
+    <t>New OPD mental health conditions</t>
+  </si>
+  <si>
+    <t>Snake Bites</t>
+  </si>
+  <si>
+    <t>WcDWC41StU4</t>
+  </si>
+  <si>
+    <t>Number of snake bites cases seen in OPD</t>
+  </si>
+  <si>
+    <t>snake_bites</t>
+  </si>
+  <si>
+    <t>egePEON9p3V</t>
+  </si>
+  <si>
+    <t>Dog Bites</t>
+  </si>
+  <si>
+    <t>Number of dog bites cases seen in OPD</t>
+  </si>
+  <si>
+    <t>dog_bites</t>
+  </si>
+  <si>
+    <t>MoH 751 Baby Friendly Community Initiative (BFCI) Community Health Unit Summary Tool</t>
+  </si>
+  <si>
+    <t>bfci_rr</t>
+  </si>
+  <si>
+    <t>aRxatsLqjce</t>
+  </si>
+  <si>
+    <t>fcdrr_rr</t>
   </si>
 </sst>
 </file>
@@ -2142,10 +2253,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40340C5E-3CDC-4A53-A0EB-1EAC89ADC307}">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -2170,7 +2281,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -2538,10 +2649,10 @@
         <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>401</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>400</v>
       </c>
       <c r="E23" s="1">
         <v>0.25</v>
@@ -2549,16 +2660,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>402</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>399</v>
       </c>
       <c r="E24" s="1">
         <v>0.25</v>
@@ -2566,16 +2677,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>401</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>400</v>
       </c>
       <c r="E25" s="1">
         <v>0.25</v>
@@ -2583,16 +2694,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>401</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>400</v>
       </c>
       <c r="E26" s="1">
         <v>0.25</v>
@@ -2600,16 +2711,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" t="s">
         <v>66</v>
-      </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>68</v>
       </c>
       <c r="E27" s="1">
         <v>0.5</v>
@@ -2617,16 +2728,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E28" s="1">
         <v>0.5</v>
@@ -2634,16 +2745,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" t="s">
         <v>71</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>72</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
       </c>
       <c r="E29" s="1">
         <v>0.25</v>
@@ -2651,16 +2762,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="1">
         <v>0.25</v>
@@ -2668,16 +2779,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" t="s">
         <v>77</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>78</v>
-      </c>
-      <c r="C31" t="s">
-        <v>79</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
       </c>
       <c r="E31" s="1">
         <v>0.25</v>
@@ -2685,16 +2796,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E32" s="1">
         <v>0.25</v>
@@ -2702,16 +2813,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E33" s="1">
         <v>0.25</v>
@@ -2719,16 +2830,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E34" s="1">
         <v>0.25</v>
@@ -2736,16 +2847,16 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>427</v>
       </c>
       <c r="D35" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E35" s="1">
         <v>0.25</v>
@@ -2753,16 +2864,16 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>427</v>
       </c>
       <c r="D36" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="E36" s="1">
         <v>0.25</v>
@@ -2770,16 +2881,16 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
         <v>94</v>
-      </c>
-      <c r="B37" t="s">
-        <v>95</v>
-      </c>
-      <c r="C37" t="s">
-        <v>96</v>
-      </c>
-      <c r="D37" t="s">
-        <v>97</v>
       </c>
       <c r="E37" s="1">
         <v>0.25</v>
@@ -2787,16 +2898,16 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
         <v>98</v>
-      </c>
-      <c r="B38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" t="s">
-        <v>101</v>
       </c>
       <c r="E38" s="1">
         <v>0.25</v>
@@ -2804,16 +2915,16 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E39" s="1">
         <v>0.25</v>
@@ -2821,16 +2932,16 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E40" s="1">
         <v>0.25</v>
@@ -2838,16 +2949,16 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C41" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E41" s="1">
         <v>0.25</v>
@@ -2855,16 +2966,16 @@
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
+        <v>105</v>
+      </c>
+      <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" t="s">
         <v>108</v>
-      </c>
-      <c r="B42" t="s">
-        <v>109</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D42" t="s">
-        <v>111</v>
       </c>
       <c r="E42" s="1">
         <v>0.25</v>
@@ -2872,16 +2983,16 @@
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D43" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="E43" s="1">
         <v>0.25</v>
@@ -2889,16 +3000,16 @@
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" t="s">
+        <v>113</v>
+      </c>
+      <c r="D44" t="s">
         <v>114</v>
-      </c>
-      <c r="B44" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" t="s">
-        <v>117</v>
       </c>
       <c r="E44" s="1">
         <v>0.25</v>
@@ -2906,16 +3017,16 @@
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>116</v>
+      </c>
+      <c r="C45" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" t="s">
         <v>118</v>
-      </c>
-      <c r="B45" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" t="s">
-        <v>120</v>
-      </c>
-      <c r="D45" t="s">
-        <v>121</v>
       </c>
       <c r="E45" s="1">
         <v>0.25</v>
@@ -2923,16 +3034,16 @@
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D46" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E46" s="1">
         <v>0.25</v>
@@ -2940,16 +3051,16 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B47" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C47" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D47" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E47" s="1">
         <v>0.25</v>
@@ -2957,16 +3068,16 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B48" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E48" s="1">
         <v>0.25</v>
@@ -2974,16 +3085,16 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D49" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E49" s="1">
         <v>0.25</v>
@@ -2991,16 +3102,16 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D50" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E50" s="1">
         <v>0.25</v>
@@ -3008,16 +3119,16 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C51" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D51" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E51" s="1">
         <v>0.25</v>
@@ -3025,16 +3136,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C52" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E52" s="1">
         <v>0.25</v>
@@ -3042,16 +3153,16 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B53" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C53" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E53" s="1">
         <v>0.25</v>
@@ -3059,16 +3170,16 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C54" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D54" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E54" s="1">
         <v>0.25</v>
@@ -3076,16 +3187,16 @@
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E55" s="1">
         <v>0.25</v>
@@ -3093,16 +3204,16 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D56" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E56" s="1">
         <v>0.25</v>
@@ -3110,16 +3221,16 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C57" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E57" s="1">
         <v>0.25</v>
@@ -3127,16 +3238,16 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C58" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E58" s="1">
         <v>0.25</v>
@@ -3144,16 +3255,16 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E59" s="1">
         <v>0.25</v>
@@ -3161,16 +3272,16 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="B60" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E60" s="1">
         <v>0.25</v>
@@ -3178,16 +3289,16 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D61" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="E61" s="1">
         <v>0.25</v>
@@ -3195,13 +3306,13 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D62" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E62" s="1">
         <v>0.25</v>
@@ -3209,13 +3320,13 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B63" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D63" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E63" s="1">
         <v>0.25</v>
@@ -3223,13 +3334,13 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B64" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D64" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E64" s="1">
         <v>0.25</v>
@@ -3237,16 +3348,13 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B65" t="s">
-        <v>172</v>
-      </c>
-      <c r="C65" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D65" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E65" s="1">
         <v>0.25</v>
@@ -3254,13 +3362,13 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B66" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D66" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E66" s="1">
         <v>0.25</v>
@@ -3268,13 +3376,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>178</v>
+        <v>300</v>
       </c>
       <c r="B67" t="s">
-        <v>179</v>
+        <v>301</v>
+      </c>
+      <c r="C67" t="s">
+        <v>174</v>
       </c>
       <c r="D67" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E67" s="1">
         <v>0.25</v>
@@ -3282,16 +3393,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B68" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C68" t="s">
-        <v>181</v>
+        <v>304</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E68" s="1">
         <v>0.25</v>
@@ -3299,16 +3410,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>309</v>
+        <v>176</v>
       </c>
       <c r="B69" t="s">
-        <v>310</v>
+        <v>177</v>
       </c>
       <c r="C69" t="s">
-        <v>311</v>
+        <v>178</v>
       </c>
       <c r="D69" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E69" s="1">
         <v>0.25</v>
@@ -3316,16 +3427,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
+        <v>180</v>
+      </c>
+      <c r="B70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70" t="s">
+        <v>182</v>
+      </c>
+      <c r="D70" t="s">
         <v>183</v>
-      </c>
-      <c r="B70" t="s">
-        <v>184</v>
-      </c>
-      <c r="C70" t="s">
-        <v>185</v>
-      </c>
-      <c r="D70" t="s">
-        <v>186</v>
       </c>
       <c r="E70" s="1">
         <v>0.25</v>
@@ -3333,16 +3444,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
+        <v>184</v>
+      </c>
+      <c r="B71" t="s">
+        <v>185</v>
+      </c>
+      <c r="C71" t="s">
+        <v>186</v>
+      </c>
+      <c r="D71" t="s">
         <v>187</v>
-      </c>
-      <c r="B71" t="s">
-        <v>188</v>
-      </c>
-      <c r="C71" t="s">
-        <v>189</v>
-      </c>
-      <c r="D71" t="s">
-        <v>190</v>
       </c>
       <c r="E71" s="1">
         <v>0.25</v>
@@ -3350,16 +3461,16 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
+        <v>188</v>
+      </c>
+      <c r="B72" t="s">
+        <v>189</v>
+      </c>
+      <c r="C72" t="s">
+        <v>190</v>
+      </c>
+      <c r="D72" t="s">
         <v>191</v>
-      </c>
-      <c r="B72" t="s">
-        <v>192</v>
-      </c>
-      <c r="C72" t="s">
-        <v>193</v>
-      </c>
-      <c r="D72" t="s">
-        <v>194</v>
       </c>
       <c r="E72" s="1">
         <v>0.25</v>
@@ -3367,16 +3478,16 @@
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
+        <v>192</v>
+      </c>
+      <c r="B73" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" t="s">
+        <v>194</v>
+      </c>
+      <c r="D73" t="s">
         <v>195</v>
-      </c>
-      <c r="B73" t="s">
-        <v>196</v>
-      </c>
-      <c r="C73" t="s">
-        <v>197</v>
-      </c>
-      <c r="D73" t="s">
-        <v>198</v>
       </c>
       <c r="E73" s="1">
         <v>0.25</v>
@@ -3384,16 +3495,16 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
+        <v>196</v>
+      </c>
+      <c r="B74" t="s">
+        <v>197</v>
+      </c>
+      <c r="C74" t="s">
+        <v>198</v>
+      </c>
+      <c r="D74" t="s">
         <v>199</v>
-      </c>
-      <c r="B74" t="s">
-        <v>200</v>
-      </c>
-      <c r="C74" t="s">
-        <v>201</v>
-      </c>
-      <c r="D74" t="s">
-        <v>202</v>
       </c>
       <c r="E74" s="1">
         <v>0.25</v>
@@ -3401,16 +3512,16 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
+        <v>200</v>
+      </c>
+      <c r="B75" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" t="s">
+        <v>202</v>
+      </c>
+      <c r="D75" t="s">
         <v>203</v>
-      </c>
-      <c r="B75" t="s">
-        <v>204</v>
-      </c>
-      <c r="C75" t="s">
-        <v>205</v>
-      </c>
-      <c r="D75" t="s">
-        <v>206</v>
       </c>
       <c r="E75" s="1">
         <v>0.25</v>
@@ -3418,16 +3529,16 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
+        <v>204</v>
+      </c>
+      <c r="B76" t="s">
+        <v>205</v>
+      </c>
+      <c r="C76" t="s">
+        <v>206</v>
+      </c>
+      <c r="D76" t="s">
         <v>207</v>
-      </c>
-      <c r="B76" t="s">
-        <v>208</v>
-      </c>
-      <c r="C76" t="s">
-        <v>209</v>
-      </c>
-      <c r="D76" t="s">
-        <v>210</v>
       </c>
       <c r="E76" s="1">
         <v>0.25</v>
@@ -3435,16 +3546,16 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B77" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C77" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D77" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E77" s="1">
         <v>0.25</v>
@@ -3452,16 +3563,16 @@
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B78" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="C78" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D78" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E78" s="1">
         <v>0.25</v>
@@ -3469,16 +3580,16 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B79" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C79" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D79" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E79" s="1">
         <v>0.25</v>
@@ -3486,16 +3597,16 @@
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B80" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D80" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E80" s="1">
         <v>0.25</v>
@@ -3503,16 +3614,16 @@
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B81" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="C81" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D81" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E81" s="1">
         <v>0.25</v>
@@ -3520,16 +3631,16 @@
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B82" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C82" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D82" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E82" s="1">
         <v>0.25</v>
@@ -3537,16 +3648,16 @@
     </row>
     <row r="83" spans="1:5">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B83" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="C83" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="D83" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="E83" s="1">
         <v>0.25</v>
@@ -3554,16 +3665,16 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B84" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C84" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="D84" t="s">
-        <v>214</v>
+        <v>225</v>
       </c>
       <c r="E84" s="1">
         <v>0.25</v>
@@ -3571,16 +3682,16 @@
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B85" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C85" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D85" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E85" s="1">
         <v>0.25</v>
@@ -3588,16 +3699,16 @@
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B86" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="C86" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D86" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E86" s="1">
         <v>0.25</v>
@@ -3605,16 +3716,16 @@
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="B87" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="C87" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D87" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E87" s="1">
         <v>0.25</v>
@@ -3622,16 +3733,16 @@
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B88" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C88" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D88" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E88" s="1">
         <v>0.25</v>
@@ -3639,16 +3750,16 @@
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="B89" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="C89" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D89" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E89" s="1">
         <v>0.25</v>
@@ -3656,16 +3767,16 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>241</v>
+        <v>330</v>
       </c>
       <c r="B90" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="C90" t="s">
-        <v>231</v>
+        <v>352</v>
       </c>
       <c r="D90" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="E90" s="1">
         <v>0.25</v>
@@ -3673,16 +3784,16 @@
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>337</v>
+        <v>350</v>
       </c>
       <c r="B91" t="s">
-        <v>243</v>
+        <v>351</v>
       </c>
       <c r="C91" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D91" t="s">
-        <v>244</v>
+        <v>354</v>
       </c>
       <c r="E91" s="1">
         <v>0.25</v>
@@ -3690,16 +3801,16 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>357</v>
+        <v>238</v>
       </c>
       <c r="B92" t="s">
-        <v>358</v>
+        <v>239</v>
       </c>
       <c r="C92" t="s">
-        <v>360</v>
+        <v>240</v>
       </c>
       <c r="D92" t="s">
-        <v>361</v>
+        <v>241</v>
       </c>
       <c r="E92" s="1">
         <v>0.25</v>
@@ -3707,16 +3818,16 @@
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
+        <v>242</v>
+      </c>
+      <c r="B93" t="s">
+        <v>243</v>
+      </c>
+      <c r="C93" t="s">
+        <v>244</v>
+      </c>
+      <c r="D93" t="s">
         <v>245</v>
-      </c>
-      <c r="B93" t="s">
-        <v>246</v>
-      </c>
-      <c r="C93" t="s">
-        <v>247</v>
-      </c>
-      <c r="D93" t="s">
-        <v>248</v>
       </c>
       <c r="E93" s="1">
         <v>0.25</v>
@@ -3724,16 +3835,16 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B94" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C94" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D94" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E94" s="1">
         <v>0.25</v>
@@ -3741,16 +3852,16 @@
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="B95" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C95" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D95" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E95" s="1">
         <v>0.25</v>
@@ -3758,16 +3869,16 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C96" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D96" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E96" s="1">
         <v>0.25</v>
@@ -3775,16 +3886,16 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B97" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C97" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D97" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E97" s="1">
         <v>0.25</v>
@@ -3792,16 +3903,16 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B98" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="C98" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="D98" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="E98" s="1">
         <v>0.25</v>
@@ -3809,16 +3920,16 @@
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="C99" t="s">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c r="D99" t="s">
-        <v>252</v>
+        <v>291</v>
       </c>
       <c r="E99" s="1">
         <v>0.25</v>
@@ -3826,13 +3937,13 @@
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B100" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="C100" t="s">
-        <v>279</v>
+        <v>299</v>
       </c>
       <c r="D100" t="s">
         <v>298</v>
@@ -3843,16 +3954,16 @@
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B101" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="C101" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D101" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="E101" s="1">
         <v>0.25</v>
@@ -3860,16 +3971,16 @@
     </row>
     <row r="102" spans="1:5">
       <c r="A102" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B102" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C102" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="D102" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="E102" s="1">
         <v>0.25</v>
@@ -3877,16 +3988,16 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="B103" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="C103" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="D103" t="s">
-        <v>316</v>
+        <v>170</v>
       </c>
       <c r="E103" s="1">
         <v>0.25</v>
@@ -3894,16 +4005,16 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="B104" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="C104" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D104" t="s">
-        <v>177</v>
+        <v>311</v>
       </c>
       <c r="E104" s="1">
         <v>0.25</v>
@@ -3911,16 +4022,16 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="B105" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C105" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D105" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E105" s="1">
         <v>0.25</v>
@@ -3928,16 +4039,16 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="B106" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C106" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="D106" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E106" s="1">
         <v>0.25</v>
@@ -3945,16 +4056,16 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" t="s">
-        <v>303</v>
+        <v>317</v>
       </c>
       <c r="B107" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C107" t="s">
         <v>322</v>
       </c>
       <c r="D107" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E107" s="1">
         <v>0.25</v>
@@ -3962,16 +4073,16 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B108" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="C108" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="D108" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="E108" s="1">
         <v>0.25</v>
@@ -3979,16 +4090,16 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B109" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C109" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D109" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="E109" s="1">
         <v>0.25</v>
@@ -3996,16 +4107,16 @@
     </row>
     <row r="110" spans="1:5">
       <c r="A110" t="s">
+        <v>326</v>
+      </c>
+      <c r="B110" t="s">
+        <v>327</v>
+      </c>
+      <c r="C110" t="s">
+        <v>332</v>
+      </c>
+      <c r="D110" t="s">
         <v>331</v>
-      </c>
-      <c r="B110" t="s">
-        <v>332</v>
-      </c>
-      <c r="C110" t="s">
-        <v>339</v>
-      </c>
-      <c r="D110" t="s">
-        <v>338</v>
       </c>
       <c r="E110" s="1">
         <v>0.25</v>
@@ -4013,16 +4124,16 @@
     </row>
     <row r="111" spans="1:5">
       <c r="A111" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B111" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C111" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D111" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="E111" s="1">
         <v>0.25</v>
@@ -4033,13 +4144,13 @@
         <v>335</v>
       </c>
       <c r="B112" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C112" t="s">
         <v>339</v>
       </c>
       <c r="D112" t="s">
-        <v>338</v>
+        <v>357</v>
       </c>
       <c r="E112" s="1">
         <v>0.25</v>
@@ -4047,16 +4158,16 @@
     </row>
     <row r="113" spans="1:5">
       <c r="A113" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B113" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="C113" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D113" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="E113" s="1">
         <v>0.25</v>
@@ -4064,16 +4175,16 @@
     </row>
     <row r="114" spans="1:5">
       <c r="A114" t="s">
-        <v>343</v>
+        <v>89</v>
       </c>
       <c r="B114" t="s">
-        <v>341</v>
+        <v>90</v>
       </c>
       <c r="C114" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D114" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
       <c r="E114" s="1">
         <v>0.25</v>
@@ -4081,16 +4192,16 @@
     </row>
     <row r="115" spans="1:5">
       <c r="A115" t="s">
-        <v>92</v>
+        <v>338</v>
       </c>
       <c r="B115" t="s">
-        <v>93</v>
+        <v>337</v>
       </c>
       <c r="C115" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D115" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E115" s="1">
         <v>0.25</v>
@@ -4098,16 +4209,16 @@
     </row>
     <row r="116" spans="1:5">
       <c r="A116" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B116" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C116" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D116" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="E116" s="1">
         <v>0.25</v>
@@ -4115,16 +4226,16 @@
     </row>
     <row r="117" spans="1:5">
       <c r="A117" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B117" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="C117" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D117" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="E117" s="1">
         <v>0.25</v>
@@ -4132,16 +4243,16 @@
     </row>
     <row r="118" spans="1:5">
       <c r="A118" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B118" t="s">
+        <v>342</v>
+      </c>
+      <c r="C118" t="s">
+        <v>349</v>
+      </c>
+      <c r="D118" t="s">
         <v>348</v>
-      </c>
-      <c r="C118" t="s">
-        <v>356</v>
-      </c>
-      <c r="D118" t="s">
-        <v>355</v>
       </c>
       <c r="E118" s="1">
         <v>0.25</v>
@@ -4149,16 +4260,16 @@
     </row>
     <row r="119" spans="1:5">
       <c r="A119" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="B119" t="s">
+        <v>346</v>
+      </c>
+      <c r="C119" t="s">
         <v>349</v>
       </c>
-      <c r="C119" t="s">
-        <v>356</v>
-      </c>
       <c r="D119" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="E119" s="1">
         <v>0.25</v>
@@ -4166,24 +4277,126 @@
     </row>
     <row r="120" spans="1:5">
       <c r="A120" t="s">
-        <v>354</v>
+        <v>403</v>
       </c>
       <c r="B120" t="s">
-        <v>353</v>
+        <v>404</v>
       </c>
       <c r="C120" t="s">
-        <v>356</v>
+        <v>405</v>
       </c>
       <c r="D120" t="s">
-        <v>355</v>
+        <v>406</v>
       </c>
       <c r="E120" s="1">
         <v>0.25</v>
       </c>
     </row>
+    <row r="121" spans="1:5">
+      <c r="A121" t="s">
+        <v>407</v>
+      </c>
+      <c r="B121" t="s">
+        <v>408</v>
+      </c>
+      <c r="C121" t="s">
+        <v>409</v>
+      </c>
+      <c r="D121" t="s">
+        <v>410</v>
+      </c>
+      <c r="E121" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5">
+      <c r="A122" t="s">
+        <v>412</v>
+      </c>
+      <c r="B122" t="s">
+        <v>411</v>
+      </c>
+      <c r="C122" t="s">
+        <v>413</v>
+      </c>
+      <c r="D122" t="s">
+        <v>414</v>
+      </c>
+      <c r="E122" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" t="s">
+        <v>416</v>
+      </c>
+      <c r="B123" t="s">
+        <v>415</v>
+      </c>
+      <c r="C123" t="s">
+        <v>417</v>
+      </c>
+      <c r="D123" t="s">
+        <v>418</v>
+      </c>
+      <c r="E123" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" t="s">
+        <v>429</v>
+      </c>
+      <c r="B124" t="s">
+        <v>428</v>
+      </c>
+      <c r="C124" t="s">
+        <v>430</v>
+      </c>
+      <c r="D124" t="s">
+        <v>167</v>
+      </c>
+      <c r="E124" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" t="s">
+        <v>432</v>
+      </c>
+      <c r="B125" t="s">
+        <v>431</v>
+      </c>
+      <c r="C125" t="s">
+        <v>433</v>
+      </c>
+      <c r="D125" t="s">
+        <v>434</v>
+      </c>
+      <c r="E125" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" t="s">
+        <v>435</v>
+      </c>
+      <c r="B126" t="s">
+        <v>436</v>
+      </c>
+      <c r="C126" t="s">
+        <v>437</v>
+      </c>
+      <c r="D126" t="s">
+        <v>438</v>
+      </c>
+      <c r="E126" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A120">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  <conditionalFormatting sqref="A1:A119 B125 A121:A127">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4194,7 +4407,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4221,113 +4434,113 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B3" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="D3" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B4" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="D6" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="D7" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="B8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="D8" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B9" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>282</v>
+      </c>
+      <c r="B10" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" t="s">
         <v>289</v>
-      </c>
-      <c r="B10" t="s">
-        <v>288</v>
-      </c>
-      <c r="D10" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B11" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="D11" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
     </row>
   </sheetData>
@@ -4337,10 +4550,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC9EE57-D82E-4B8F-978D-34E9C6B04B8F}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4355,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -4363,123 +4576,167 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="B4" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C4" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B5" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B7" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B8" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B9" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B10" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B11" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="B12" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>402</v>
+        <v>395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>419</v>
+      </c>
+      <c r="B13" t="s">
+        <v>420</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>422</v>
+      </c>
+      <c r="B14" t="s">
+        <v>421</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>425</v>
+      </c>
+      <c r="B15" t="s">
+        <v>424</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>441</v>
+      </c>
+      <c r="B16" t="s">
+        <v>439</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor indicators to dynamic generic module
Replaces vaccine-specific modules with a dynamic generic indicator module driven by a new get_indicators() function. Updates UI and server logic to generate indicator panels programmatically, adds support for analysis type selection, and enhances indicator calculations and display. Removes vaccine modules and related code, updates data preparation scripts, and adds new internal datasets and tests.
</commit_message>
<xml_diff>
--- a/inst/indicators.xlsx
+++ b/inst/indicators.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\R\moh.analytics\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFDCC4A-9B28-4D36-B5CA-07A69AE89747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7687F86D-555E-43D2-A6F6-D5E5B620B624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="1830" windowWidth="13116" windowHeight="8904" xr2:uid="{6387D201-81FB-42D9-A202-087F66466527}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{6387D201-81FB-42D9-A202-087F66466527}"/>
   </bookViews>
   <sheets>
     <sheet name="service" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,16 @@
     <sheet name="datasets" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="451">
   <si>
     <t>element_id</t>
   </si>
@@ -1351,6 +1356,30 @@
   </si>
   <si>
     <t>fcdrr_rr</t>
+  </si>
+  <si>
+    <t>IHlMRYVhmOX</t>
+  </si>
+  <si>
+    <t>madOGCuPg8q</t>
+  </si>
+  <si>
+    <t>f0SJMmqh8un</t>
+  </si>
+  <si>
+    <t>MOH 711 Stunting 0-&lt;6 months</t>
+  </si>
+  <si>
+    <t>MOH 711 Stunting 24-59 Months</t>
+  </si>
+  <si>
+    <t>MOH 711 Stunting 6-23 months</t>
+  </si>
+  <si>
+    <t>&lt;5yrs who are stunted</t>
+  </si>
+  <si>
+    <t>stunted</t>
   </si>
 </sst>
 </file>
@@ -1859,7 +1888,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1867,6 +1896,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2253,10 +2283,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40340C5E-3CDC-4A53-A0EB-1EAC89ADC307}">
-  <dimension ref="A1:E126"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4394,8 +4424,59 @@
         <v>0.25</v>
       </c>
     </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="B127" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D127" t="s">
+        <v>450</v>
+      </c>
+      <c r="E127" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="B128" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D128" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="E128" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="5" t="s">
+        <v>445</v>
+      </c>
+      <c r="B129" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C129" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="E129" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A119 B125 A121:A127">
+  <conditionalFormatting sqref="A1:A119 B125 A121:A126 A127:C129">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>